<commit_message>
Can define a style directly in a cell
</commit_message>
<xml_diff>
--- a/test/xlsx/oneRow.xlsx
+++ b/test/xlsx/oneRow.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nullam aliquet mi et nunc tempus rutrum.</t>
   </si>
@@ -19,10 +19,25 @@
     <t>__proto__</t>
   </si>
   <si>
+    <t>Labore duis cillum dolor adipisicing cillum dolore.</t>
+  </si>
+  <si>
     <t>Dolore anim</t>
   </si>
   <si>
     <t>not date</t>
+  </si>
+  <si>
+    <t>Irure duis sit cupidatat culpa adipisicing nisi.</t>
+  </si>
+  <si>
+    <t>Ullamco cillum</t>
+  </si>
+  <si>
+    <t>Est sunt esse elit reprehenderit exercitation irure.</t>
+  </si>
+  <si>
+    <t>Culpa occaecat</t>
   </si>
 </sst>
 </file>
@@ -32,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$ #,##0.00;$ #,##0.00;-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font/>
     <font>
       <b/>
@@ -43,6 +58,9 @@
       <i/>
       <color rgb="FFFF0000"/>
     </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -61,6 +79,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkHorizontal">
+        <fgColor rgb="FF008800"/>
+        <bgColor rgb="FF000088"/>
       </patternFill>
     </fill>
     <fill>
@@ -72,12 +96,6 @@
           <color rgb="FF5B9BD5"/>
         </stop>
       </gradientFill>
-    </fill>
-    <fill>
-      <patternFill patternType="darkHorizontal">
-        <fgColor rgb="FF008800"/>
-        <bgColor rgb="FF000088"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -104,19 +122,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf/>
     <xf applyAlignment="true" numFmtId="164" applyNumberFormat="true" fontId="1" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf fillId="3" applyFill="true"/>
+    <xf applyProtection="true" fontId="2" applyFont="true" fillId="3" applyFill="true">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf fillId="4" applyFill="true"/>
     <xf numFmtId="164" applyNumberFormat="true"/>
     <xf applyAlignment="true" numFmtId="14" applyNumberFormat="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf applyProtection="true" fontId="2" applyFont="true" fillId="4" applyFill="true">
-      <protection locked="0" hidden="1"/>
-    </xf>
+    <xf fontId="3" applyFont="true"/>
   </cellXfs>
   <dxfs count="0"/>
 </styleSheet>
@@ -130,86 +149,86 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" customWidth="1" width="10"/>
-    <col min="2" max="2" customWidth="1" width="40" style="format2"/>
-    <col min="3" max="3" width="9.140625" style="format3"/>
-    <col min="4" max="4" width="9.140625"/>
-    <col min="5" max="5" customWidth="1" width="12" style="format4"/>
+    <col min="2" max="2" customWidth="1" width="50" style="3"/>
+    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" customWidth="1" width="15"/>
+    <col min="5" max="5" customWidth="1" width="12" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" ht="30" customFormat="1" s="5">
+    <row r="1" customHeight="1" ht="30" customFormat="1" s="2">
       <c r="A1" s="1">
         <v>2541</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="2">
         <v>260</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5">
-        <v>41105.8449537037</v>
-      </c>
-      <c r="F1" s="5">
-        <v>41112.8449537037</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" ht="30" customFormat="1" s="null" outlineLevel="1">
+      <c r="E1" s="2">
+        <v>41105.8449537037</v>
+      </c>
+      <c r="F1" s="2">
+        <v>41112.8449537037</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" ht="25" outlineLevel="1">
       <c r="A2" s="1">
         <v>2541</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>260</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="4">
+        <v>205</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="F2">
         <v>41112.8449537037</v>
       </c>
     </row>
-    <row r="3" customHeight="1" ht="30" customFormat="1" s="null">
+    <row r="3" customHeight="1" ht="20">
       <c r="A3" s="1">
         <v>2541</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>260</v>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5">
         <v>41105.8449537037</v>
       </c>
       <c r="F3">
         <v>41112.8449537037</v>
       </c>
     </row>
-    <row r="4" customHeight="1" ht="30" customFormat="1" s="null">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="1">
         <v>2541</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>260</v>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
         <v>41105.8449537037</v>
       </c>
       <c r="F4">
@@ -218,41 +237,41 @@
     </row>
     <row r="5"/>
     <row r="6"/>
-    <row r="7" customHeight="1" ht="30" customFormat="1" s="5">
+    <row r="7" customHeight="1" ht="30" customFormat="1" s="2">
       <c r="A7" s="1">
         <v>2541</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>260</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
-        <v>41105.8449537037</v>
-      </c>
-      <c r="F7" s="5">
-        <v>41112.8449537037</v>
-      </c>
-    </row>
-    <row r="8" customFormat="1" s="null" outlineLevel="1">
+      <c r="E7" s="2">
+        <v>41105.8449537037</v>
+      </c>
+      <c r="F7" s="2">
+        <v>41112.8449537037</v>
+      </c>
+    </row>
+    <row r="8" outlineLevel="1">
       <c r="A8" s="1">
         <v>2541</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>260</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="C8" s="4">
+        <v>205</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>3</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="F8">
         <v>41112.8449537037</v>
@@ -262,16 +281,16 @@
       <c r="A9" s="1">
         <v>2541</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>260</v>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5">
         <v>41105.8449537037</v>
       </c>
       <c r="F9">
@@ -282,16 +301,16 @@
       <c r="A10" s="1">
         <v>2541</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>260</v>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5">
         <v>41105.8449537037</v>
       </c>
       <c r="F10">

</xml_diff>

<commit_message>
Merge cell, row and column styles for each cell
</commit_message>
<xml_diff>
--- a/test/xlsx/oneRow.xlsx
+++ b/test/xlsx/oneRow.xlsx
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$ #,##0.00;$ #,##0.00;-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font/>
     <font>
       <b/>
@@ -60,6 +60,12 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <u/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="5">
@@ -83,8 +89,8 @@
     </fill>
     <fill>
       <patternFill patternType="darkHorizontal">
-        <fgColor rgb="FF008800"/>
-        <bgColor rgb="FF000088"/>
+        <fgColor rgb="FF88FF88"/>
+        <bgColor rgb="FF8888F0"/>
       </patternFill>
     </fill>
     <fill>
@@ -122,7 +128,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf/>
     <xf applyAlignment="true" numFmtId="164" applyNumberFormat="true" fontId="1" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true">
       <alignment horizontal="center"/>
@@ -135,7 +141,11 @@
     <xf applyAlignment="true" numFmtId="14" applyNumberFormat="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf fontId="3" applyFont="true"/>
+    <xf numFmtId="164" applyNumberFormat="true" fontId="3" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true"/>
+    <xf fontId="2" applyFont="true" fillId="3" applyFill="true"/>
+    <xf numFmtId="164" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true"/>
+    <xf numFmtId="14" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true"/>
+    <xf fontId="4" applyFont="true"/>
   </cellXfs>
   <dxfs count="0"/>
 </styleSheet>
@@ -156,19 +166,19 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" ht="30" customFormat="1" s="2">
-      <c r="A1" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="6">
+        <v>2541</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="8">
         <v>260</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="9">
         <v>41105.8449537037</v>
       </c>
       <c r="F1" s="2">
@@ -185,7 +195,7 @@
       <c r="C2" s="4">
         <v>205</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -238,19 +248,19 @@
     <row r="5"/>
     <row r="6"/>
     <row r="7" customHeight="1" ht="30" customFormat="1" s="2">
-      <c r="A7" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6">
+        <v>2541</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>260</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="9">
         <v>41105.8449537037</v>
       </c>
       <c r="F7" s="2">
@@ -267,7 +277,7 @@
       <c r="C8" s="4">
         <v>205</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="5" t="s">

</xml_diff>

<commit_message>
Fixed the styles merge
</commit_message>
<xml_diff>
--- a/test/xlsx/oneRow.xlsx
+++ b/test/xlsx/oneRow.xlsx
@@ -104,7 +104,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,13 +127,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF8888FF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellXfs count="11">
     <xf/>
     <xf applyAlignment="true" numFmtId="164" applyNumberFormat="true" fontId="1" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyProtection="true" fontId="2" applyFont="true" fillId="3" applyFill="true">
+    <xf applyProtection="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true">
       <protection locked="0" hidden="1"/>
     </xf>
     <xf fillId="4" applyFill="true"/>
@@ -142,9 +151,9 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="164" applyNumberFormat="true" fontId="3" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true"/>
-    <xf fontId="2" applyFont="true" fillId="3" applyFill="true"/>
-    <xf numFmtId="164" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true"/>
-    <xf numFmtId="14" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true"/>
+    <xf fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
+    <xf numFmtId="164" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
+    <xf numFmtId="14" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
     <xf fontId="4" applyFont="true"/>
   </cellXfs>
   <dxfs count="0"/>

</xml_diff>

<commit_message>
Styles merge was refactored
</commit_message>
<xml_diff>
--- a/test/xlsx/oneRow.xlsx
+++ b/test/xlsx/oneRow.xlsx
@@ -68,7 +68,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none">
         <fgColor rgb="FFFFFFFF"/>
@@ -102,6 +102,12 @@
           <color rgb="FF5B9BD5"/>
         </stop>
       </gradientFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -151,7 +157,7 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="164" applyNumberFormat="true" fontId="3" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true"/>
-    <xf fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
+    <xf fontId="2" applyFont="true" fillId="5" applyFill="true" borderId="2" applyBorder="true"/>
     <xf numFmtId="164" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
     <xf numFmtId="14" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
     <xf fontId="4" applyFont="true"/>

</xml_diff>

<commit_message>
Not fill rows and columns by default
</commit_message>
<xml_diff>
--- a/test/xlsx/oneRow.xlsx
+++ b/test/xlsx/oneRow.xlsx
@@ -62,7 +62,7 @@
       <b/>
       <i/>
       <u/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
     </font>
     <font>
       <b/>
@@ -110,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,8 +142,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF8888FF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf/>
     <xf applyAlignment="true" numFmtId="164" applyNumberFormat="true" fontId="1" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true">
       <alignment horizontal="center"/>
@@ -151,15 +166,18 @@
     <xf applyProtection="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true">
       <protection locked="0" hidden="1"/>
     </xf>
+    <xf numFmtId="164" applyNumberFormat="true" fontId="1" applyFont="true"/>
     <xf fillId="4" applyFill="true"/>
     <xf numFmtId="164" applyNumberFormat="true"/>
     <xf applyAlignment="true" numFmtId="14" applyNumberFormat="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="true" fontId="3" applyFont="true" fillId="2" applyFill="true" borderId="1" applyBorder="true"/>
+    <xf numFmtId="14" applyNumberFormat="true"/>
+    <xf numFmtId="164" applyNumberFormat="true" fontId="3" applyFont="true" fillId="3" applyFill="true" borderId="3" applyBorder="true"/>
     <xf fontId="2" applyFont="true" fillId="5" applyFill="true" borderId="2" applyBorder="true"/>
     <xf numFmtId="164" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
     <xf numFmtId="14" applyNumberFormat="true" fontId="2" applyFont="true" fillId="3" applyFill="true" borderId="2" applyBorder="true"/>
+    <xf fontId="2" applyFont="true"/>
     <xf fontId="4" applyFont="true"/>
   </cellXfs>
   <dxfs count="0"/>
@@ -173,27 +191,27 @@
     <sheetView workbookViewId="0" view="normal"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="10"/>
-    <col min="2" max="2" customWidth="1" width="50" style="3"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
+    <col min="1" max="1" customWidth="1" width="10" style="3"/>
+    <col min="2" max="2" customWidth="1" width="50" style="4"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
     <col min="4" max="4" customWidth="1" width="15"/>
-    <col min="5" max="5" customWidth="1" width="12" style="5"/>
+    <col min="5" max="5" customWidth="1" width="12" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" ht="30" customFormat="1" s="2">
-      <c r="A1" s="6">
+    <row r="1" customHeight="1" ht="30" customFormat="1" s="12">
+      <c r="A1" s="8">
         <v>2541</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8">
+      <c r="C1" s="10">
         <v>260</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="11">
         <v>41105.8449537037</v>
       </c>
       <c r="F1" s="2">
@@ -202,18 +220,18 @@
     </row>
     <row r="2" customHeight="1" ht="25" outlineLevel="1">
       <c r="A2" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B2" s="3" t="s">
+        <v>2542</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>205</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F2">
@@ -222,18 +240,18 @@
     </row>
     <row r="3" customHeight="1" ht="20">
       <c r="A3" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>41105.8449537037</v>
       </c>
       <c r="F3">
@@ -242,18 +260,18 @@
     </row>
     <row r="4" customHeight="1" ht="15">
       <c r="A4" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>2544</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>145</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>41105.8449537037</v>
       </c>
       <c r="F4">
@@ -262,20 +280,20 @@
     </row>
     <row r="5"/>
     <row r="6"/>
-    <row r="7" customHeight="1" ht="30" customFormat="1" s="2">
-      <c r="A7" s="6">
+    <row r="7" customHeight="1" ht="30" customFormat="1" s="12">
+      <c r="A7" s="8">
         <v>2541</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="10">
         <v>260</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="11">
         <v>41105.8449537037</v>
       </c>
       <c r="F7" s="2">
@@ -284,18 +302,18 @@
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>2542</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>205</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F8">
@@ -304,18 +322,18 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>41105.8449537037</v>
       </c>
       <c r="F9">
@@ -324,18 +342,18 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>2541</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>2544</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>145</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <v>41105.8449537037</v>
       </c>
       <c r="F10">

</xml_diff>

<commit_message>
Preserve spaces in strings
</commit_message>
<xml_diff>
--- a/test/xlsx/oneRow.xlsx
+++ b/test/xlsx/oneRow.xlsx
@@ -31,13 +31,13 @@
     <t>Irure duis sit cupidatat culpa adipisicing nisi.</t>
   </si>
   <si>
-    <t>Ullamco cillum</t>
+    <t xml:space="preserve"> String with header space</t>
   </si>
   <si>
     <t>Est sunt esse elit reprehenderit exercitation irure.</t>
   </si>
   <si>
-    <t>Culpa occaecat</t>
+    <t xml:space="preserve">String with trailing space </t>
   </si>
 </sst>
 </file>
@@ -194,7 +194,7 @@
     <col min="1" max="1" customWidth="1" width="10" style="3"/>
     <col min="2" max="2" customWidth="1" width="50" style="4"/>
     <col min="3" max="3" width="9.140625" style="5"/>
-    <col min="4" max="4" customWidth="1" width="15"/>
+    <col min="4" max="4" customWidth="1" width="25"/>
     <col min="5" max="5" customWidth="1" width="12" style="7"/>
   </cols>
   <sheetData>

</xml_diff>